<commit_message>
started binary trees question
</commit_message>
<xml_diff>
--- a/love_babbar_FINAL450.xlsx
+++ b/love_babbar_FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS Code\C++\love-babbar-dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A0D2EC-BDB4-4B3C-A2D0-601513B7BB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E3DAC2-1B22-4974-850F-8941B7664082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,6 +1426,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -1857,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="C180" sqref="C180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2007,7 +2010,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21">
@@ -2018,7 +2021,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21">
@@ -2029,7 +2032,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21">
@@ -3699,7 +3702,7 @@
         <v>172</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="21">
@@ -3710,7 +3713,7 @@
         <v>173</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="21">
@@ -3721,7 +3724,7 @@
         <v>174</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="21">

</xml_diff>

<commit_message>
commiting changes to excel
</commit_message>
<xml_diff>
--- a/love_babbar_FINAL450.xlsx
+++ b/love_babbar_FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS Code\C++\love-babbar-dsa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeBase\C++\love-babbar-dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5C91F9-BBA1-4D62-B341-7474120DF5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEC7060-FA41-47BD-AECC-B6FD0F92CE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2043,7 +2043,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21">
@@ -2054,7 +2054,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21">
@@ -2065,7 +2065,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="21">
@@ -2076,7 +2076,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21">
@@ -2087,7 +2087,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21">
@@ -2098,7 +2098,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="21">
@@ -2290,16 +2290,12 @@
     </row>
     <row r="42" spans="1:3" ht="21">
       <c r="B42" s="7"/>
-      <c r="C42" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:3" ht="21">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
-      <c r="C43" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C43" s="4"/>
     </row>
     <row r="44" spans="1:3" ht="21">
       <c r="A44" s="8" t="s">
@@ -3302,7 +3298,7 @@
         <v>135</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="21">
@@ -3735,7 +3731,7 @@
         <v>175</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="21">
@@ -3746,7 +3742,7 @@
         <v>176</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="21">
@@ -3757,7 +3753,7 @@
         <v>177</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="21">
@@ -3768,7 +3764,7 @@
         <v>178</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="21">
@@ -3779,7 +3775,7 @@
         <v>179</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="21">
@@ -3790,7 +3786,7 @@
         <v>180</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="21">
@@ -3801,7 +3797,7 @@
         <v>181</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="21">
@@ -3812,7 +3808,7 @@
         <v>182</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="21">
@@ -3823,7 +3819,7 @@
         <v>183</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="21">
@@ -3834,7 +3830,7 @@
         <v>184</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="21">
@@ -3845,7 +3841,7 @@
         <v>185</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="21">

</xml_diff>

<commit_message>
updates on array questions code
</commit_message>
<xml_diff>
--- a/love_babbar_FINAL450.xlsx
+++ b/love_babbar_FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeBase\C++\Revision-Questions\love-babbar-dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A1C7B6-8E62-4B6A-AE09-F47C6048A7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744C3DAA-F464-4621-AE00-60A171EE6188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1498,7 +1498,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1511,13 +1511,34 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1552,7 +1573,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1872,8 +1893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1905,7 +1926,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="21">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -1927,7 +1948,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -1938,7 +1959,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -1993,7 +2014,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -2004,7 +2025,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="21">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="6" t="s">

</xml_diff>